<commit_message>
Adding adding items to cart & checkout test cases
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7500"/>
+    <workbookView windowWidth="20490" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CardInformation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +58,24 @@
   </si>
   <si>
     <t>Invalid</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>ExpDate</t>
+  </si>
+  <si>
+    <t>GiftCard</t>
+  </si>
+  <si>
+    <t>CreditCard</t>
   </si>
 </sst>
 </file>
@@ -672,8 +691,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -996,7 +1015,7 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1018,10 +1037,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -1029,7 +1048,7 @@
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -1040,7 +1059,7 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -1048,7 +1067,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1093,4 +1112,68 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="11.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="12.8571428571429"/>
+    <col min="4" max="4" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>98990988877</v>
+      </c>
+      <c r="C2">
+        <v>202</v>
+      </c>
+      <c r="D2" s="1">
+        <v>46266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>58455544115</v>
+      </c>
+      <c r="C3">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1">
+        <v>47481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>